<commit_message>
payment functionality completed by Anil
payment functionality completed by Anil
</commit_message>
<xml_diff>
--- a/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
+++ b/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anil Kumar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>ContractId</t>
   </si>
@@ -163,12 +163,21 @@
   </si>
   <si>
     <t>AirForce</t>
+  </si>
+  <si>
+    <t>BCD0019</t>
+  </si>
+  <si>
+    <t>BCD0013</t>
+  </si>
+  <si>
+    <t>BCD0015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,31 +503,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" customWidth="1"/>
+    <col min="18" max="18" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -571,10 +581,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>C2</f>
-        <v>DFER2545</v>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -609,6 +618,9 @@
       <c r="L2" s="2">
         <v>3</v>
       </c>
+      <c r="M2">
+        <v>1000</v>
+      </c>
       <c r="N2" t="s">
         <v>22</v>
       </c>
@@ -622,10 +634,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>C3</f>
-        <v>DFER2545</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
@@ -660,6 +671,9 @@
       <c r="L3" s="2">
         <v>3</v>
       </c>
+      <c r="M3">
+        <v>1000</v>
+      </c>
       <c r="N3" t="s">
         <v>22</v>
       </c>
@@ -673,10 +687,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>C4</f>
-        <v>DFER2545</v>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
@@ -710,6 +723,9 @@
       </c>
       <c r="L4" s="2">
         <v>3</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
       </c>
       <c r="N4" t="s">
         <v>22</v>
@@ -738,25 +754,25 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -800,10 +816,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Sheet1!A2</f>
-        <v>DFER2545</v>
+        <v>BCD0013</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -845,10 +861,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Sheet1!A2</f>
-        <v>DFER2545</v>
+        <v>BCD0013</v>
       </c>
       <c r="B3">
         <v>2</v>

</xml_diff>

<commit_message>
Anil changes after payment module testing.
Anil changes after payment module testing.
</commit_message>
<xml_diff>
--- a/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
+++ b/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anil Kumar\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>ContractId</t>
   </si>
@@ -82,18 +77,6 @@
   </si>
   <si>
     <t>this is category</t>
-  </si>
-  <si>
-    <t>this is Incoterms</t>
-  </si>
-  <si>
-    <t>3 months</t>
-  </si>
-  <si>
-    <t>Hi this is ny duties</t>
-  </si>
-  <si>
-    <t>Hi this is contents</t>
   </si>
   <si>
     <t>Services</t>
@@ -177,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -316,7 +299,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -493,47 +476,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.88671875" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18.109375" customWidth="1"/>
-    <col min="18" max="18" width="28.5546875" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -581,12 +564,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -600,46 +583,22 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1">
-        <v>44288</v>
-      </c>
-      <c r="H2" s="1">
-        <v>44288</v>
-      </c>
-      <c r="I2" s="2">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>44288</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2">
-        <v>3</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="M2">
         <v>1000</v>
       </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
       <c r="P2" s="1">
         <v>44288</v>
       </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -653,46 +612,22 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1">
-        <v>44288</v>
-      </c>
-      <c r="H3" s="1">
-        <v>44288</v>
-      </c>
-      <c r="I3" s="2">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1">
-        <v>44288</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2">
-        <v>3</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="M3">
         <v>1000</v>
       </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
       <c r="P3" s="1">
         <v>44288</v>
       </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -706,38 +641,14 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="H4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="I4" s="2">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2">
-        <v>3</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
       <c r="M4">
         <v>1000</v>
       </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
       <c r="P4" s="1">
         <v>44288</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -747,76 +658,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="28.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" t="str">
         <f>Sheet1!A2</f>
         <v>BCD0013</v>
@@ -825,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>44295</v>
@@ -843,25 +754,25 @@
         <v>44295</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1">
         <v>44295</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1">
         <v>44295</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" t="str">
         <f>Sheet1!A2</f>
         <v>BCD0013</v>
@@ -870,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1">
         <v>44295</v>
@@ -888,22 +799,22 @@
         <v>44295</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1">
         <v>44295</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L3" s="1">
         <v>44295</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contract payment changes on 20-04-21
Contract payment changes on 20-04-21
</commit_message>
<xml_diff>
--- a/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
+++ b/Src/ACQ.Web.App/ExcelFile/ContractMaster.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>ContractId</t>
   </si>
@@ -70,15 +75,24 @@
     <t>GracePeriod</t>
   </si>
   <si>
-    <t>DFER2545</t>
-  </si>
-  <si>
     <t>Hi, This is Description</t>
   </si>
   <si>
     <t>this is category</t>
   </si>
   <si>
+    <t>this is Incoterms</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>Hi this is ny duties</t>
+  </si>
+  <si>
+    <t>Hi this is contents</t>
+  </si>
+  <si>
     <t>Services</t>
   </si>
   <si>
@@ -142,26 +156,17 @@
     <t>yes</t>
   </si>
   <si>
-    <t>navy</t>
-  </si>
-  <si>
-    <t>AirForce</t>
-  </si>
-  <si>
-    <t>BCD0019</t>
-  </si>
-  <si>
-    <t>BCD0013</t>
-  </si>
-  <si>
-    <t>BCD0015</t>
+    <t>BCDNO17</t>
+  </si>
+  <si>
+    <t>BCDID17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -299,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -476,21 +481,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
@@ -508,15 +513,15 @@
     <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="19.7109375" customWidth="1"/>
     <col min="17" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="28.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -564,91 +569,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>44288</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1">
+        <v>44288</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44288</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44288</v>
+      </c>
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="L2" s="2">
+        <v>3</v>
+      </c>
       <c r="M2">
-        <v>1000</v>
+        <v>5000</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
       </c>
       <c r="P2" s="1">
         <v>44288</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="P3" s="1">
-        <v>44288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="M4">
-        <v>1000</v>
-      </c>
-      <c r="P4" s="1">
-        <v>44288</v>
+      <c r="Q2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -658,14 +629,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -683,60 +654,60 @@
     <col min="14" max="14" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Sheet1!A2</f>
-        <v>BCD0013</v>
+        <v>BCDID17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>44295</v>
@@ -754,34 +725,34 @@
         <v>44295</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1">
         <v>44295</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L2" s="1">
         <v>44295</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>Sheet1!A2</f>
-        <v>BCD0013</v>
+        <v>BCDID17</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>44295</v>
@@ -799,22 +770,22 @@
         <v>44295</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1">
         <v>44295</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L3" s="1">
         <v>44295</v>
       </c>
       <c r="M3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>